<commit_message>
correct linreg uptakes stderr
</commit_message>
<xml_diff>
--- a/data/GrowthRates/RatesCompare.xlsx
+++ b/data/GrowthRates/RatesCompare.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -86,7 +86,13 @@
     <t xml:space="preserve">Growth-Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Growth-Rate-Std</t>
+  </si>
+  <si>
     <t xml:space="preserve">Substrate-uptake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uptake-Std</t>
   </si>
   <si>
     <t xml:space="preserve">2229v1</t>
@@ -125,6 +131,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -227,7 +234,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -325,102 +332,138 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>3</v>
+      <c r="D2" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>0.86</v>
       </c>
+      <c r="F3" s="1" t="n">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>0.82</v>
       </c>
+      <c r="F4" s="1" t="n">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="C6" s="1" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
+      <c r="E6" s="1" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
update growth rate analysis
</commit_message>
<xml_diff>
--- a/data/GrowthRates/RatesCompare.xlsx
+++ b/data/GrowthRates/RatesCompare.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -95,12 +95,18 @@
     <t xml:space="preserve">Uptake-Std</t>
   </si>
   <si>
+    <t xml:space="preserve">Rct-Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">2229v1</t>
   </si>
   <si>
     <t xml:space="preserve">10-30</t>
   </si>
   <si>
+    <t xml:space="preserve">EX_glc__D_e</t>
+  </si>
+  <si>
     <t xml:space="preserve">LV3_130_v1</t>
   </si>
   <si>
@@ -111,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">LV3_200_v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100-200</t>
   </si>
   <si>
     <t xml:space="preserve">LV3_200_v2</t>
@@ -234,7 +237,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -332,13 +335,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -359,33 +362,39 @@
       <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1.53</v>
+        <v>0.49</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.86</v>
+        <v>0.14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.07</v>
@@ -399,13 +408,16 @@
       <c r="F3" s="1" t="n">
         <v>0.22</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.07</v>
@@ -419,33 +431,39 @@
       <c r="F4" s="1" t="n">
         <v>0.27</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C5" s="1" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="E5" s="1" t="n">
-        <v>0.1</v>
+        <v>1.06</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0.02</v>
+        <v>0.38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.06</v>
@@ -458,6 +476,9 @@
       </c>
       <c r="F6" s="1" t="n">
         <v>0.44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
memote 2601, rates+biolog corrections
</commit_message>
<xml_diff>
--- a/data/GrowthRates/RatesCompare.xlsx
+++ b/data/GrowthRates/RatesCompare.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -140,19 +140,28 @@
     <t xml:space="preserve">log</t>
   </si>
   <si>
-    <t xml:space="preserve">LV3_130_v1</t>
+    <t xml:space="preserve">LV3_130v1</t>
   </si>
   <si>
     <t xml:space="preserve">0-300</t>
   </si>
   <si>
-    <t xml:space="preserve">LV3_130_v2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV3_200_v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV3_200_v2</t>
+    <t xml:space="preserve">LV3_130v2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV3_200v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV3_200v2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV11_glc20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lin</t>
   </si>
   <si>
     <t xml:space="preserve">Wierckx_50glc</t>
@@ -276,10 +285,10 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="H7 E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -288,7 +297,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -482,13 +491,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -647,54 +656,80 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E7" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="E7" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>1.24</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>0.34</v>
+      <c r="F7" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.12</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>45</v>
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>0.67</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.19</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update GAM, NGAM Figure growth
</commit_message>
<xml_diff>
--- a/data/GrowthRates/RatesCompare.xlsx
+++ b/data/GrowthRates/RatesCompare.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t xml:space="preserve">Metadata: Key</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t xml:space="preserve">0-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB215</t>
   </si>
   <si>
     <t xml:space="preserve">Wierckx_100glc</t>
@@ -174,8 +177,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -249,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -259,6 +263,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,7 +297,7 @@
       <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -417,13 +429,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.83"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -432,37 +447,40 @@
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -473,37 +491,40 @@
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="G2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>0.18</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="J2" s="1" t="n">
         <v>0.97</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>2.2</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>0.89</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>0.45</v>
       </c>
     </row>
@@ -514,37 +535,40 @@
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="G3" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.97</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>1.1</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="L3" s="1" t="n">
         <v>0.34</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="M3" s="1" t="n">
         <v>0.95</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="N3" s="1" t="n">
         <v>0.33</v>
       </c>
     </row>
@@ -555,37 +579,40 @@
       <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="G4" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.96</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.74</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="L4" s="1" t="n">
         <v>0.18</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="M4" s="1" t="n">
         <v>0.96</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="N4" s="1" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -596,37 +623,40 @@
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="G5" s="1" t="n">
         <v>203</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="J5" s="1" t="n">
         <v>0.96</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>0.33</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.98</v>
       </c>
-      <c r="M5" s="1" t="n">
+      <c r="N5" s="1" t="n">
         <v>0.33</v>
       </c>
     </row>
@@ -637,37 +667,40 @@
       <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="G6" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="H6" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="I6" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="J6" s="1" t="n">
         <v>0.74</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="K6" s="1" t="n">
         <v>0.36</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="L6" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="M6" s="1" t="n">
         <v>0.98</v>
       </c>
-      <c r="M6" s="1" t="n">
+      <c r="N6" s="1" t="n">
         <v>0.33</v>
       </c>
     </row>
@@ -678,160 +711,172 @@
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="G7" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="H7" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="I7" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="J7" s="1" t="n">
         <v>0.98</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="K7" s="1" t="n">
         <v>1.22</v>
       </c>
-      <c r="K7" s="1" t="n">
+      <c r="L7" s="1" t="n">
         <v>0.36</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="M7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M7" s="1" t="n">
+      <c r="N7" s="1" t="n">
         <v>0.36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="G8" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="H8" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="I8" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="J8" s="1" t="n">
         <v>0.83</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="K8" s="1" t="n">
         <v>0.67</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="L8" s="1" t="n">
         <v>0.19</v>
       </c>
-      <c r="L8" s="1" t="n">
+      <c r="M8" s="1" t="n">
         <v>0.99</v>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="N8" s="1" t="n">
         <v>0.33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="G9" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="H9" s="1" t="n">
         <v>0.27</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="I9" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="J9" s="1" t="n">
         <v>0.99</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="K9" s="1" t="n">
         <v>6.24</v>
       </c>
-      <c r="K9" s="1" t="n">
+      <c r="L9" s="1" t="n">
         <v>1.17</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="M9" s="1" t="n">
         <v>0.99</v>
       </c>
-      <c r="M9" s="1" t="n">
+      <c r="N9" s="1" t="n">
         <v>0.24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>521</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="1" t="n">
         <v>1.97</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="H10" s="1" t="n">
         <v>0.02</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="I10" s="1" t="n">
         <v>0.004</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="J10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="K10" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="L10" s="1" t="n">
         <v>0.004</v>
       </c>
-      <c r="L10" s="1" t="n">
+      <c r="M10" s="1" t="n">
         <v>0.92</v>
       </c>
-      <c r="M10" s="1" t="n">
+      <c r="N10" s="1" t="n">
         <v>21.74</v>
       </c>
     </row>

</xml_diff>